<commit_message>
Cleanup old results for Frontiers submission
</commit_message>
<xml_diff>
--- a/QTL_results/LOD_peaks_Lentil_FT13038_Homozyg_V1_snps_mapping_30_06_2021.xlsx
+++ b/QTL_results/LOD_peaks_Lentil_FT13038_Homozyg_V1_snps_mapping_30_06_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1bd5\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/Supervision/Hari/QTL_analysis/QTL_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_0D8EEE85B1F823B4A531FC3BD513C367B6DFA983" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0D8EEE85B1F823B4A531FC3BD513C367B6DFA983" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0E84B49-9692-454D-8A99-CB6622041902}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOD_peaks" sheetId="1" r:id="rId1"/>
@@ -126,6 +126,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:H13" totalsRowShown="0">
   <autoFilter ref="A1:H13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
+    <sortCondition ref="E1:E13"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="lodindex"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="lodcolumn"/>
@@ -476,45 +479,45 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>87.486456227114601</v>
       </c>
       <c r="E2">
-        <v>2.7382344539915699</v>
+        <v>2.5805159842311198</v>
       </c>
       <c r="F2">
-        <v>19.353835123049802</v>
+        <v>79.958827907516607</v>
       </c>
       <c r="G2">
-        <v>94.141824956588593</v>
+        <v>94.141822956588697</v>
       </c>
       <c r="H2">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>51.5009060070361</v>
+        <v>90</v>
       </c>
       <c r="E3">
-        <v>3.6970809677616701</v>
+        <v>2.64916906074252</v>
       </c>
       <c r="F3">
-        <v>44.452941804791003</v>
+        <v>22.0714172420093</v>
       </c>
       <c r="G3">
-        <v>55.619716073830297</v>
+        <v>94.141822956588697</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,16 +534,16 @@
         <v>51.947347442036197</v>
       </c>
       <c r="E4">
-        <v>2.8645964548859801</v>
+        <v>2.659005886309</v>
       </c>
       <c r="F4">
-        <v>31.048011794482601</v>
+        <v>29.330870976658499</v>
       </c>
       <c r="G4">
         <v>57.502740308639702</v>
       </c>
       <c r="H4">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -557,68 +560,68 @@
         <v>90</v>
       </c>
       <c r="E5">
-        <v>3.0685405333657099</v>
+        <v>2.7382344539915699</v>
       </c>
       <c r="F5">
-        <v>79.958827907516607</v>
+        <v>19.353835123049802</v>
       </c>
       <c r="G5">
-        <v>94.141822956588697</v>
+        <v>94.141824956588593</v>
       </c>
       <c r="H5">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>51.5009060070361</v>
+        <v>51.947347442036197</v>
       </c>
       <c r="E6">
-        <v>3.4273614336079499</v>
+        <v>2.8645964548859801</v>
       </c>
       <c r="F6">
-        <v>34.095660304742601</v>
+        <v>31.048011794482601</v>
       </c>
       <c r="G6">
-        <v>55.619716073830297</v>
+        <v>57.502740308639702</v>
       </c>
       <c r="H6">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>35.965693631810097</v>
+        <v>41.036047334005502</v>
       </c>
       <c r="E7">
-        <v>3.1807381549921998</v>
+        <v>2.8725301605989699</v>
       </c>
       <c r="F7">
-        <v>29.330870976658499</v>
+        <v>25.793529080343799</v>
       </c>
       <c r="G7">
-        <v>55.619716073830297</v>
+        <v>42.569622515955899</v>
       </c>
       <c r="H7">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -632,10 +635,10 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>87.486456227114601</v>
+        <v>90</v>
       </c>
       <c r="E8">
-        <v>2.5805159842311198</v>
+        <v>3.0685405333657099</v>
       </c>
       <c r="F8">
         <v>79.958827907516607</v>
@@ -644,33 +647,33 @@
         <v>94.141822956588697</v>
       </c>
       <c r="H8">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>45.307726923498002</v>
+        <v>35.965693631810097</v>
       </c>
       <c r="E9">
-        <v>3.28799963199365</v>
+        <v>3.1807381549921998</v>
       </c>
       <c r="F9">
-        <v>34.095660304742601</v>
+        <v>29.330870976658499</v>
       </c>
       <c r="G9">
-        <v>52.8908566416074</v>
+        <v>55.619716073830297</v>
       </c>
       <c r="H9">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -681,19 +684,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>41.036047334005502</v>
+        <v>45.307726923498002</v>
       </c>
       <c r="E10">
-        <v>2.8725301605989699</v>
+        <v>3.28799963199365</v>
       </c>
       <c r="F10">
-        <v>25.793529080343799</v>
+        <v>34.095660304742601</v>
       </c>
       <c r="G10">
-        <v>42.569622515955899</v>
+        <v>52.8908566416074</v>
       </c>
       <c r="H10">
         <v>28</v>
@@ -701,25 +704,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>51.947347442036197</v>
+        <v>49.539108620998697</v>
       </c>
       <c r="E11">
-        <v>2.659005886309</v>
+        <v>3.4159023155010799</v>
       </c>
       <c r="F11">
-        <v>29.330870976658499</v>
+        <v>34.095660304742601</v>
       </c>
       <c r="G11">
-        <v>57.502740308639702</v>
+        <v>55.619716073830297</v>
       </c>
       <c r="H11">
         <v>28</v>
@@ -727,54 +730,54 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>90</v>
+        <v>51.5009060070361</v>
       </c>
       <c r="E12">
-        <v>2.64916906074252</v>
+        <v>3.4273614336079499</v>
       </c>
       <c r="F12">
-        <v>22.0714172420093</v>
+        <v>34.095660304742601</v>
       </c>
       <c r="G12">
-        <v>94.141822956588697</v>
+        <v>55.619716073830297</v>
       </c>
       <c r="H12">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13">
-        <v>49.539108620998697</v>
+        <v>51.5009060070361</v>
       </c>
       <c r="E13">
-        <v>3.4159023155010799</v>
+        <v>3.6970809677616701</v>
       </c>
       <c r="F13">
-        <v>34.095660304742601</v>
+        <v>44.452941804791003</v>
       </c>
       <c r="G13">
         <v>55.619716073830297</v>
       </c>
       <c r="H13">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>